<commit_message>
Added slug shotguns to damage test, Added buyability of resources, Added upkeep mechanic
</commit_message>
<xml_diff>
--- a/other-stuff/Raided.xlsx
+++ b/other-stuff/Raided.xlsx
@@ -8,26 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viddie\Desktop\git\RustInfos\other-stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053F7B4F-4329-4363-83DA-8767722198E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7B2BAD-E234-4971-B419-3DE662F3B7CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -39,7 +30,7 @@
     <author>viddie</author>
   </authors>
   <commentList>
-    <comment ref="L7" authorId="0" shapeId="0" xr:uid="{971A2CA2-401E-441B-85B2-AA35A68BFEF6}">
+    <comment ref="M7" authorId="0" shapeId="0" xr:uid="{971A2CA2-401E-441B-85B2-AA35A68BFEF6}">
       <text>
         <r>
           <rPr>
@@ -60,6 +51,31 @@
             <family val="2"/>
           </rPr>
           <t>Ignores Explo Ammo Cost</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{A32010BC-B241-4284-A5BD-411E0E4F157A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>viddie:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Softsided:
+3x Metal Wall</t>
         </r>
       </text>
     </comment>
@@ -147,7 +163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K10" authorId="0" shapeId="0" xr:uid="{25F525DE-BEEB-422A-BBFE-59A20B34B411}">
+    <comment ref="L10" authorId="0" shapeId="0" xr:uid="{25F525DE-BEEB-422A-BBFE-59A20B34B411}">
       <text>
         <r>
           <rPr>
@@ -192,6 +208,158 @@
           </rPr>
           <t xml:space="preserve">
 Pixel gap loot room was first present in this raid</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{034680CE-BDB5-4974-B231-FA2BC70CEBFE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>viddie:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Softsided:
+3x Stone Wall</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J11" authorId="0" shapeId="0" xr:uid="{45A59B55-31ED-4FDA-95DD-AC1571AFAD0A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>viddie:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1x Stone Wall
+1x HQ Wall
+--------------------
+19x Rockets</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{3971CC7C-FA8C-45EC-ACCF-F90F5E07A067}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>viddie:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+From this base forward this bunker doesn't exist anymore</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{801D5711-9B0D-498C-B4E4-0C1BE7D20BB9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>viddie:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+From this base forward there are 2 pixel gap loot rooms</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{9A443751-4ACB-4B17-9524-315FAA1ECF5F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>viddie:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+From this base forward multi-TC is used to prevent griefing</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J12" authorId="0" shapeId="0" xr:uid="{32116C05-778E-4F0A-9956-869BC5FC7F12}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>viddie:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1x Stone Wall
+6x Garage Door
+1x Sheet Metal Door
+------------------
+17x Rockets + 254x Explo Ammo</t>
         </r>
       </text>
     </comment>
@@ -200,7 +368,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>How often &amp; severe were we raided</t>
   </si>
@@ -223,9 +391,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>Est. shit loot</t>
-  </si>
-  <si>
     <t>Est. Rockets</t>
   </si>
   <si>
@@ -272,6 +437,15 @@
   </si>
   <si>
     <t>Kinda</t>
+  </si>
+  <si>
+    <t>N / N</t>
+  </si>
+  <si>
+    <t>Est. Explo Ammo</t>
+  </si>
+  <si>
+    <t>Est. Shit Loot</t>
   </si>
 </sst>
 </file>
@@ -279,8 +453,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0\+"/>
-    <numFmt numFmtId="166" formatCode="\~0"/>
+    <numFmt numFmtId="164" formatCode="0\+"/>
+    <numFmt numFmtId="165" formatCode="\~0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -453,6 +627,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -462,11 +641,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -749,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:Q22"/>
+  <dimension ref="C2:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,68 +936,61 @@
     <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="19" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C3" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="O3" s="16" t="s">
+    <row r="2" spans="3:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="P4" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+    </row>
+    <row r="5" spans="3:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="P5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-    </row>
-    <row r="4" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="O4" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="R5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="Q4" s="14" t="s">
+    </row>
+    <row r="6" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="P6" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="3:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="O5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P5" s="2">
+      <c r="Q6" s="2">
         <v>4</v>
       </c>
-      <c r="Q5" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="O6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P6" s="3">
-        <v>8</v>
-      </c>
-      <c r="Q6" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="R6" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
@@ -834,37 +1001,40 @@
         <v>3</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="M7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q7" s="3">
         <v>8</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P7" s="3">
-        <v>15</v>
-      </c>
-      <c r="Q7" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="R7" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C8" s="4">
         <v>44263</v>
       </c>
@@ -886,27 +1056,30 @@
       <c r="I8" s="8">
         <v>0.4</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="17">
         <v>35</v>
       </c>
-      <c r="K8" s="22">
+      <c r="K8" s="17">
+        <v>0</v>
+      </c>
+      <c r="L8" s="19">
         <v>3000</v>
       </c>
-      <c r="L8" s="2">
-        <f>J8*1400-K8</f>
+      <c r="M8" s="2">
+        <f>J8*1400-L8+K8*25</f>
         <v>46000</v>
       </c>
-      <c r="O8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P8" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="12">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="P8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>15</v>
+      </c>
+      <c r="R8" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C9" s="6">
         <v>44267</v>
       </c>
@@ -928,27 +1101,30 @@
       <c r="I9" s="7">
         <v>1</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="18">
         <v>46</v>
       </c>
-      <c r="K9" s="23">
+      <c r="K9" s="18">
+        <v>98</v>
+      </c>
+      <c r="L9" s="20">
         <v>8000</v>
       </c>
-      <c r="L9" s="3">
-        <f>J9*1400-K9</f>
-        <v>56400</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P9" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q9" s="12">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="M9" s="3">
+        <f>J9*1400-L9+K9*25</f>
+        <v>58850</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>1</v>
+      </c>
+      <c r="R9" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C10" s="6">
         <v>44269</v>
       </c>
@@ -965,56 +1141,113 @@
         <v>4</v>
       </c>
       <c r="H10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="16">
+        <v>0.25</v>
+      </c>
+      <c r="J10" s="18">
+        <v>43</v>
+      </c>
+      <c r="K10" s="18">
+        <v>98</v>
+      </c>
+      <c r="L10" s="20">
+        <v>6000</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" ref="M10:M22" si="0">J10*1400-L10+K10*25</f>
+        <v>56650</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>2</v>
+      </c>
+      <c r="R10" s="12">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C11" s="6">
+        <v>44274</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="16">
+        <v>0.05</v>
+      </c>
+      <c r="J11" s="18">
+        <v>19</v>
+      </c>
+      <c r="K11" s="18">
+        <v>0</v>
+      </c>
+      <c r="L11" s="20">
+        <v>0</v>
+      </c>
+      <c r="M11" s="3">
+        <f t="shared" si="0"/>
+        <v>26600</v>
+      </c>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="12"/>
+    </row>
+    <row r="12" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C12" s="6">
+        <v>44286</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="19">
-        <v>0.25</v>
-      </c>
-      <c r="J10" s="21">
-        <v>43</v>
-      </c>
-      <c r="K10" s="23">
-        <v>6000</v>
-      </c>
-      <c r="L10" s="3">
-        <f>J10*1400-K10</f>
-        <v>54200</v>
-      </c>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="12"/>
-    </row>
-    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="12"/>
-    </row>
-    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="3"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="13"/>
-    </row>
-    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="G12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="J12" s="18">
+        <v>17</v>
+      </c>
+      <c r="K12" s="18">
+        <v>254</v>
+      </c>
+      <c r="L12" s="20">
+        <v>1000</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" si="0"/>
+        <v>29150</v>
+      </c>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="12"/>
+    </row>
+    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1022,11 +1255,18 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="3"/>
-    </row>
-    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="13"/>
+    </row>
+    <row r="14" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -1034,11 +1274,15 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="3"/>
-    </row>
-    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1046,11 +1290,15 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="3"/>
-    </row>
-    <row r="16" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -1058,11 +1306,15 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="3"/>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -1070,11 +1322,15 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1082,11 +1338,15 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="3"/>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1094,11 +1354,15 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -1106,11 +1370,15 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="3"/>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -1118,11 +1386,15 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="3"/>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -1130,13 +1402,17 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="3"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="P4:R4"/>
     <mergeCell ref="C3:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added resource images, Added more buyable resources & prettified it
</commit_message>
<xml_diff>
--- a/other-stuff/Raided.xlsx
+++ b/other-stuff/Raided.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viddie\Desktop\git\RustInfos\other-stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7B2BAD-E234-4971-B419-3DE662F3B7CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AADF2445-31B4-49B6-8864-E1F47F9705F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -363,12 +363,63 @@
         </r>
       </text>
     </comment>
+    <comment ref="J13" authorId="0" shapeId="0" xr:uid="{F14C002B-51C7-4A99-9B1A-D3CCE760E915}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>viddie:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+8x Garage Door
+4x Sheet Metal Door
+------------------
+20x Rockets + 360x Explo Ammo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L13" authorId="0" shapeId="0" xr:uid="{B67C1003-D38B-44B7-8D6C-78FACEBCA8C8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>viddie:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+After tilting we didn't move the GP into the Bunker and left it in the unsecured chests.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="30">
   <si>
     <t>How often &amp; severe were we raided</t>
   </si>
@@ -446,6 +497,18 @@
   </si>
   <si>
     <t>Est. Shit Loot</t>
+  </si>
+  <si>
+    <t>Trio 2</t>
+  </si>
+  <si>
+    <t>Odd</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Rocket deficit</t>
   </si>
 </sst>
 </file>
@@ -610,7 +673,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -640,6 +703,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -923,10 +992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:R22"/>
+  <dimension ref="B2:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,35 +1009,36 @@
     <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="19" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.5703125" customWidth="1"/>
     <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C3" s="22" t="s">
-        <v>0</v>
-      </c>
+    <row r="2" spans="2:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
       <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-    </row>
-    <row r="4" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="23"/>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
       <c r="P4" s="21" t="s">
         <v>12</v>
       </c>
       <c r="Q4" s="21"/>
       <c r="R4" s="21"/>
     </row>
-    <row r="5" spans="3:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="P5" s="1" t="s">
         <v>13</v>
       </c>
@@ -979,7 +1049,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="P6" s="2" t="s">
         <v>16</v>
       </c>
@@ -990,7 +1060,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1024,6 +1097,9 @@
       <c r="M7" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="N7" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="P7" s="3" t="s">
         <v>17</v>
       </c>
@@ -1034,7 +1110,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="C8" s="4">
         <v>44263</v>
       </c>
@@ -1069,6 +1148,10 @@
         <f>J8*1400-L8+K8*25</f>
         <v>46000</v>
       </c>
+      <c r="N8" s="24">
+        <f t="shared" ref="N8:N12" si="0">IF(ROUND(M8/1400*(-1),2)&gt;0,CONCATENATE("+",ROUND(M8/1400*(-1),2)),ROUND(M8/1400*(-1),2))</f>
+        <v>-32.86</v>
+      </c>
       <c r="P8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1079,7 +1162,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="C9" s="6">
         <v>44267</v>
       </c>
@@ -1114,6 +1200,10 @@
         <f>J9*1400-L9+K9*25</f>
         <v>58850</v>
       </c>
+      <c r="N9" s="25">
+        <f t="shared" si="0"/>
+        <v>-42.04</v>
+      </c>
       <c r="P9" s="3" t="s">
         <v>19</v>
       </c>
@@ -1124,7 +1214,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="C10" s="6">
         <v>44269</v>
       </c>
@@ -1156,8 +1249,12 @@
         <v>6000</v>
       </c>
       <c r="M10" s="3">
-        <f t="shared" ref="M10:M22" si="0">J10*1400-L10+K10*25</f>
+        <f t="shared" ref="M10:M22" si="1">J10*1400-L10+K10*25</f>
         <v>56650</v>
+      </c>
+      <c r="N10" s="25">
+        <f t="shared" si="0"/>
+        <v>-40.46</v>
       </c>
       <c r="P10" s="3" t="s">
         <v>20</v>
@@ -1169,7 +1266,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="C11" s="6">
         <v>44274</v>
       </c>
@@ -1201,14 +1301,21 @@
         <v>0</v>
       </c>
       <c r="M11" s="3">
+        <f t="shared" si="1"/>
+        <v>26600</v>
+      </c>
+      <c r="N11" s="25">
         <f t="shared" si="0"/>
-        <v>26600</v>
+        <v>-19</v>
       </c>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
       <c r="R11" s="12"/>
     </row>
-    <row r="12" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="C12" s="6">
         <v>44286</v>
       </c>
@@ -1240,49 +1347,108 @@
         <v>1000</v>
       </c>
       <c r="M12" s="3">
+        <f t="shared" si="1"/>
+        <v>29150</v>
+      </c>
+      <c r="N12" s="25">
         <f t="shared" si="0"/>
-        <v>29150</v>
+        <v>-20.82</v>
       </c>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="12"/>
     </row>
-    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="20"/>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="6">
+        <v>44290</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="16">
+        <v>1</v>
+      </c>
+      <c r="J13" s="18">
+        <v>17</v>
+      </c>
+      <c r="K13" s="18">
+        <v>360</v>
+      </c>
+      <c r="L13" s="20">
+        <v>40000</v>
+      </c>
       <c r="M13" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>-7200</v>
+      </c>
+      <c r="N13" s="25" t="str">
+        <f>IF(ROUND(M13/1400*(-1),2)&gt;0,CONCATENATE("+",ROUND(M13/1400*(-1),2)),ROUND(M13/1400*(-1),2))</f>
+        <v>+5,14</v>
       </c>
       <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
       <c r="R13" s="13"/>
     </row>
-    <row r="14" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="20"/>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="6">
+        <v>44292</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="J14" s="18">
+        <v>4</v>
+      </c>
+      <c r="K14" s="18">
+        <v>0</v>
+      </c>
+      <c r="L14" s="20">
+        <v>0</v>
+      </c>
       <c r="M14" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>5600</v>
+      </c>
+      <c r="N14" s="25">
+        <f t="shared" ref="N14:N22" si="2">IF(ROUND(M14/1400*(-1),2)&gt;0,CONCATENATE("+",ROUND(M14/1400*(-1),2)),ROUND(M14/1400*(-1),2))</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1294,11 +1460,16 @@
       <c r="K15" s="18"/>
       <c r="L15" s="20"/>
       <c r="M15" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -1310,11 +1481,16 @@
       <c r="K16" s="18"/>
       <c r="L16" s="20"/>
       <c r="M16" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -1326,11 +1502,16 @@
       <c r="K17" s="18"/>
       <c r="L17" s="20"/>
       <c r="M17" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1342,11 +1523,16 @@
       <c r="K18" s="18"/>
       <c r="L18" s="20"/>
       <c r="M18" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1358,11 +1544,16 @@
       <c r="K19" s="18"/>
       <c r="L19" s="20"/>
       <c r="M19" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -1374,11 +1565,16 @@
       <c r="K20" s="18"/>
       <c r="L20" s="20"/>
       <c r="M20" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -1390,11 +1586,16 @@
       <c r="K21" s="18"/>
       <c r="L21" s="20"/>
       <c r="M21" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -1406,14 +1607,18 @@
       <c r="K22" s="18"/>
       <c r="L22" s="20"/>
       <c r="M22" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="25">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="P4:R4"/>
-    <mergeCell ref="C3:G4"/>
+    <mergeCell ref="B3:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>